<commit_message>
bijwerken uren en groeiportfolio
</commit_message>
<xml_diff>
--- a/uren_project.xlsx
+++ b/uren_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gille\Desktop\school\2deJaar\IT-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F2C936-39D7-4B1C-A62D-797BC2A6E87E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36D3A98-18BC-44EA-A45E-8B16C10D4725}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8AEF082B-D6B0-4005-8E7F-3162498CEF5A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>opstellen beschrijving IT-project</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>basis functionaliteit toegevoegd.</t>
+  </si>
+  <si>
+    <t>oplossen problemen met Create, verschillende kleine aanpassingen aan design en views.</t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C40658E-4990-4F71-94B9-979A02492AD7}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,13 +604,25 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="2">
+        <v>44319</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C12" s="1">
-        <f>SUM(C2:C11)</f>
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1">
+        <f>SUM(C2:C12)</f>
+        <v>55</v>
+      </c>
+      <c r="D13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>